<commit_message>
OK! Added difficulty funny text.
</commit_message>
<xml_diff>
--- a/data/IART.xlsx
+++ b/data/IART.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuela\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuela\Documents\FEUP\IART_project1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E2B9F6-FE93-4C43-85E9-4340511574DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F15A52AD-DEDE-4309-8E98-9F9B135BC7D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{718CC8A0-930C-4084-B92E-FF0F35B09587}"/>
   </bookViews>
@@ -649,7 +649,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1074,6 +1073,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1926356751"/>
+        <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>

</xml_diff>